<commit_message>
Update comforter-cda daily records
</commit_message>
<xml_diff>
--- a/pakuro/pakuro-cda.xlsx
+++ b/pakuro/pakuro-cda.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{588F4407-B23C-4BAA-AB3B-31B06E75EF5E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{928C7340-8812-4710-8539-88AB26B50651}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="comforter-cda" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -32,6 +32,12 @@
   </si>
   <si>
     <t>Duration</t>
+  </si>
+  <si>
+    <t>Second Duration</t>
+  </si>
+  <si>
+    <t>Absolute Value</t>
   </si>
 </sst>
 </file>
@@ -71,20 +77,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="7">
     <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
@@ -94,6 +104,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -109,14 +122,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4F241E2-70B8-4E1C-A71D-2175999E1A36}" name="comforter_cda_table" displayName="comforter_cda_table" ref="A1:D15" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:D15" xr:uid="{60EC4219-E3F1-48A9-8A10-9A735D5CAA88}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B3194266-B947-4321-8934-F9C47FA9DE1C}" name="Date" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{3BD6ED93-E3D0-4F67-BDB8-9FEC9229AD12}" name="Start Time" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00E660B2-6437-4AE9-BEC8-C301204937AF}" name="End Time" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{D9963DBC-C69E-420B-82AB-9CD5E60E9512}" name="Duration" dataDxfId="1">
-      <calculatedColumnFormula>C2-B2</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4F241E2-70B8-4E1C-A71D-2175999E1A36}" name="comforter_cda_table" displayName="comforter_cda_table" ref="A1:F15" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:F15" xr:uid="{60EC4219-E3F1-48A9-8A10-9A735D5CAA88}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{B3194266-B947-4321-8934-F9C47FA9DE1C}" name="Date" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{3BD6ED93-E3D0-4F67-BDB8-9FEC9229AD12}" name="Start Time" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00E660B2-6437-4AE9-BEC8-C301204937AF}" name="End Time" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{D9963DBC-C69E-420B-82AB-9CD5E60E9512}" name="Duration" dataDxfId="2">
+      <calculatedColumnFormula>(C2-B2)* 1440</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{B183478E-E8AE-4F0F-833D-55D03DF9F101}" name="Second Duration" dataDxfId="1">
+      <calculatedColumnFormula>IF(C2&gt;B2, (C2-B2)*1440, (B2-C2)*1440)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{30C329C8-FEBC-46A6-984D-95D036A78306}" name="Absolute Value" dataDxfId="0">
+      <calculatedColumnFormula>ABS((C2-B2)*1440)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -386,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D15"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -397,10 +416,12 @@
     <col min="1" max="1" width="26" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -410,11 +431,17 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>43334</v>
       </c>
@@ -424,110 +451,240 @@
       <c r="C2" s="1">
         <v>0.3923611111111111</v>
       </c>
-      <c r="D2" s="1">
-        <f>C2-B2</f>
-        <v>2.083333333333337E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" s="3">
+        <f>(C2-B2)* 1440</f>
+        <v>30.000000000000053</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E15" si="0">IF(C2&gt;B2, (C2-B2)*1440, (B2-C2)*1440)</f>
+        <v>30.000000000000053</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ref="F2:F15" si="1">ABS((C2-B2)*1440)</f>
+        <v>30.000000000000053</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>0.41666666666666669</v>
       </c>
       <c r="C3" s="1">
         <v>0.42569444444444443</v>
       </c>
-      <c r="D3" s="1">
-        <f t="shared" ref="D3:D15" si="0">C3-B3</f>
-        <v>9.0277777777777457E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="3">
+        <f t="shared" ref="D3:D15" si="2">(C3-B3)* 1440</f>
+        <v>12.999999999999954</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>12.999999999999954</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="1"/>
+        <v>12.999999999999954</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>0.52083333333333337</v>
       </c>
       <c r="C4" s="1">
         <v>0.56666666666666665</v>
       </c>
-      <c r="D4" s="1">
-        <f t="shared" si="0"/>
-        <v>4.5833333333333282E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="3">
+        <f t="shared" si="2"/>
+        <v>65.999999999999929</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>65.999999999999929</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>65.999999999999929</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>0.56805555555555554</v>
       </c>
       <c r="C5" s="1">
         <v>0.72083333333333333</v>
       </c>
-      <c r="D5" s="1">
-        <f t="shared" si="0"/>
-        <v>0.15277777777777779</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5" s="3">
+        <f t="shared" si="2"/>
+        <v>220.00000000000003</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>220.00000000000003</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>220.00000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>43335</v>
       </c>
       <c r="B6" s="1">
         <v>0.78472222222222221</v>
       </c>
-      <c r="D6" s="1">
-        <f t="shared" si="0"/>
-        <v>-0.78472222222222221</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D7" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D8" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D9" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D10" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D11" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D12" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D13" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D14" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D15" s="1">
-        <f t="shared" si="0"/>
+      <c r="C6" s="1">
+        <v>0.4993055555555555</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="2"/>
+        <v>-411.00000000000006</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>411.00000000000006</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>411.00000000000006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>43336</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="2"/>
+        <v>400</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>43337</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.41180555555555554</v>
+      </c>
+      <c r="D8" s="3">
+        <f>(C8-B8)* 1440</f>
+        <v>-593</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>593</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>593</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D13" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D15" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update comforter cda records
</commit_message>
<xml_diff>
--- a/pakuro/pakuro-cda.xlsx
+++ b/pakuro/pakuro-cda.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{928C7340-8812-4710-8539-88AB26B50651}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3FEE371F-8DF2-4E39-BD45-CC97D6F7C5BC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2250" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="comforter-cda" sheetId="1" r:id="rId1"/>
@@ -408,7 +408,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,59 +577,86 @@
       <c r="B8" s="1">
         <v>0.41180555555555554</v>
       </c>
+      <c r="C8" s="1">
+        <v>0.44791666666666669</v>
+      </c>
       <c r="D8" s="3">
         <f>(C8-B8)* 1440</f>
-        <v>-593</v>
+        <v>52.000000000000057</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>593</v>
+        <v>52.000000000000057</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>593</v>
+        <v>52.000000000000057</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.71527777777777779</v>
+      </c>
       <c r="D9" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>139.99999999999997</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>139.99999999999997</v>
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>139.99999999999997</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>43338</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.78819444444444453</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.4993055555555555</v>
+      </c>
       <c r="D10" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-416.00000000000023</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>416.00000000000023</v>
       </c>
       <c r="F10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>416.00000000000023</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>43339</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.2986111111111111</v>
+      </c>
       <c r="D11" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>430</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>430</v>
       </c>
       <c r="F11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>430</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add daily record for zion cda
</commit_message>
<xml_diff>
--- a/pakuro/pakuro-cda.xlsx
+++ b/pakuro/pakuro-cda.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9E63333D-15D1-4F86-BC78-A671C0E892B9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{763F89A4-BAD6-4DFF-9C1F-E4DD5523375F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2700" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3150" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="comforter-cda" sheetId="1" r:id="rId1"/>
@@ -408,7 +408,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,6 +686,12 @@
       <c r="A13" s="2">
         <v>43341</v>
       </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
       <c r="D13" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -700,20 +706,35 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>43342</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.86111111111111116</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.99930555555555556</v>
+      </c>
       <c r="D14" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>198.99999999999994</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>198.99999999999994</v>
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>198.99999999999994</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>43343</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
       <c r="D15" s="3">
         <f t="shared" si="2"/>
         <v>0</v>

</xml_diff>

<commit_message>
Add daily cda record
</commit_message>
<xml_diff>
--- a/pakuro/pakuro-cda.xlsx
+++ b/pakuro/pakuro-cda.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0659ABAA-87B9-4511-9DB4-E88446EF6946}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{22A07140-3629-4C5A-BC28-3429152BE0A6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3600" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4050" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="comforter-cda" sheetId="1" r:id="rId1"/>
@@ -77,11 +77,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -122,8 +123,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4F241E2-70B8-4E1C-A71D-2175999E1A36}" name="comforter_cda_table" displayName="comforter_cda_table" ref="A1:F15" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:F15" xr:uid="{60EC4219-E3F1-48A9-8A10-9A735D5CAA88}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4F241E2-70B8-4E1C-A71D-2175999E1A36}" name="comforter_cda_table" displayName="comforter_cda_table" ref="A1:F17" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:F17" xr:uid="{60EC4219-E3F1-48A9-8A10-9A735D5CAA88}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B3194266-B947-4321-8934-F9C47FA9DE1C}" name="Date" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{3BD6ED93-E3D0-4F67-BDB8-9FEC9229AD12}" name="Start Time" dataDxfId="4"/>
@@ -405,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,19 +533,19 @@
         <v>0.78472222222222221</v>
       </c>
       <c r="C6" s="1">
-        <v>0.4993055555555555</v>
+        <v>0.49998842592592596</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" si="2"/>
-        <v>-411.00000000000006</v>
+        <v>-410.01666666666659</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>411.00000000000006</v>
+        <v>410.01666666666659</v>
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
-        <v>411.00000000000006</v>
+        <v>410.01666666666659</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -621,19 +622,19 @@
         <v>0.78819444444444453</v>
       </c>
       <c r="C10" s="1">
-        <v>0.4993055555555555</v>
+        <v>0.49998842592592596</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" si="2"/>
-        <v>-416.00000000000023</v>
+        <v>-415.01666666666677</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>416.00000000000023</v>
+        <v>415.01666666666677</v>
       </c>
       <c r="F10">
         <f t="shared" si="1"/>
-        <v>416.00000000000023</v>
+        <v>415.01666666666677</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -735,16 +736,62 @@
       <c r="B15" s="1">
         <v>0</v>
       </c>
+      <c r="C15" s="1">
+        <v>0.34097222222222223</v>
+      </c>
       <c r="D15" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>491</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>491</v>
       </c>
       <c r="F15">
         <f t="shared" si="1"/>
+        <v>491</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>43344</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.84166666666666667</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="D16" s="3">
+        <f>(C16-B16)* 1440</f>
+        <v>227</v>
+      </c>
+      <c r="E16" s="4">
+        <f>IF(C16&gt;B16, (C16-B16)*1440, (B16-C16)*1440)</f>
+        <v>227</v>
+      </c>
+      <c r="F16" s="4">
+        <f>ABS((C16-B16)*1440)</f>
+        <v>227</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>43345</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3">
+        <f>(C17-B17)* 1440</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="4">
+        <f>IF(C17&gt;B17, (C17-B17)*1440, (B17-C17)*1440)</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="4">
+        <f>ABS((C17-B17)*1440)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add daily power records
</commit_message>
<xml_diff>
--- a/pakuro/pakuro-cda.xlsx
+++ b/pakuro/pakuro-cda.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7EC1A017-C17A-44DA-919E-A2769BAD7A85}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B6BF1C5E-C674-4088-BEF9-1D9C43F9B16E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4500" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4950" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="comforter-cda" sheetId="1" r:id="rId1"/>
@@ -123,8 +123,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4F241E2-70B8-4E1C-A71D-2175999E1A36}" name="comforter_cda_table" displayName="comforter_cda_table" ref="A1:F20" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:F20" xr:uid="{60EC4219-E3F1-48A9-8A10-9A735D5CAA88}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4F241E2-70B8-4E1C-A71D-2175999E1A36}" name="comforter_cda_table" displayName="comforter_cda_table" ref="A1:F21" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:F21" xr:uid="{60EC4219-E3F1-48A9-8A10-9A735D5CAA88}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B3194266-B947-4321-8934-F9C47FA9DE1C}" name="Date" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{3BD6ED93-E3D0-4F67-BDB8-9FEC9229AD12}" name="Start Time" dataDxfId="4"/>
@@ -406,15 +406,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="3" bestFit="1" customWidth="1"/>
@@ -857,16 +857,45 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>43347</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.74236111111111114</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.99930555555555556</v>
+      </c>
       <c r="D20" s="3">
         <f>(C20-B20)* 1440</f>
-        <v>0</v>
+        <v>369.99999999999994</v>
       </c>
       <c r="E20" s="4">
         <f>IF(C20&gt;B20, (C20-B20)*1440, (B20-C20)*1440)</f>
-        <v>0</v>
+        <v>369.99999999999994</v>
       </c>
       <c r="F20" s="4">
         <f>ABS((C20-B20)*1440)</f>
+        <v>369.99999999999994</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>43348</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="3">
+        <f>(C21-B21)* 1440</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="4">
+        <f>IF(C21&gt;B21, (C21-B21)*1440, (B21-C21)*1440)</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="4">
+        <f>ABS((C21-B21)*1440)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update daily power records
</commit_message>
<xml_diff>
--- a/pakuro/pakuro-cda.xlsx
+++ b/pakuro/pakuro-cda.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4197DA91-7242-4274-A541-E2AC96285F7A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{13DE6DE6-CD22-4D0E-A760-1D89ABD43DA8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5850" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="6300" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="comforter-cda" sheetId="1" r:id="rId1"/>
@@ -123,8 +123,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4F241E2-70B8-4E1C-A71D-2175999E1A36}" name="comforter_cda_table" displayName="comforter_cda_table" ref="A1:F25" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:F25" xr:uid="{60EC4219-E3F1-48A9-8A10-9A735D5CAA88}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4F241E2-70B8-4E1C-A71D-2175999E1A36}" name="comforter_cda_table" displayName="comforter_cda_table" ref="A1:F27" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:F27" xr:uid="{60EC4219-E3F1-48A9-8A10-9A735D5CAA88}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B3194266-B947-4321-8934-F9C47FA9DE1C}" name="Date" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{3BD6ED93-E3D0-4F67-BDB8-9FEC9229AD12}" name="Start Time" dataDxfId="4"/>
@@ -406,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,17 +978,57 @@
       <c r="B25" s="1">
         <v>0.35069444444444442</v>
       </c>
+      <c r="C25" s="1">
+        <v>0.56805555555555554</v>
+      </c>
       <c r="D25" s="3">
         <f>(C25-B25)* 1440</f>
-        <v>-504.99999999999994</v>
+        <v>313</v>
       </c>
       <c r="E25" s="4">
         <f>IF(C25&gt;B25, (C25-B25)*1440, (B25-C25)*1440)</f>
-        <v>504.99999999999994</v>
+        <v>313</v>
       </c>
       <c r="F25" s="4">
         <f>ABS((C25-B25)*1440)</f>
-        <v>504.99999999999994</v>
+        <v>313</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>43352</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.57500000000000007</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0.72361111111111109</v>
+      </c>
+      <c r="D26" s="3">
+        <f>(C26-B26)* 1440</f>
+        <v>213.99999999999989</v>
+      </c>
+      <c r="E26" s="4">
+        <f>IF(C26&gt;B26, (C26-B26)*1440, (B26-C26)*1440)</f>
+        <v>213.99999999999989</v>
+      </c>
+      <c r="F26" s="4">
+        <f>ABS((C26-B26)*1440)</f>
+        <v>213.99999999999989</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D27" s="3">
+        <f>(C27-B27)* 1440</f>
+        <v>0</v>
+      </c>
+      <c r="E27" s="4">
+        <f>IF(C27&gt;B27, (C27-B27)*1440, (B27-C27)*1440)</f>
+        <v>0</v>
+      </c>
+      <c r="F27" s="4">
+        <f>ABS((C27-B27)*1440)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add daily power record
</commit_message>
<xml_diff>
--- a/pakuro/pakuro-cda.xlsx
+++ b/pakuro/pakuro-cda.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{828CF57E-FC33-4CD8-986F-3E3CCD5F4CD2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{60611DF8-576E-4981-94D3-076B70A6C2FA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6750" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="7200" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="comforter-cda" sheetId="1" r:id="rId1"/>
@@ -123,8 +123,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4F241E2-70B8-4E1C-A71D-2175999E1A36}" name="comforter_cda_table" displayName="comforter_cda_table" ref="A1:F30" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:F30" xr:uid="{60EC4219-E3F1-48A9-8A10-9A735D5CAA88}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4F241E2-70B8-4E1C-A71D-2175999E1A36}" name="comforter_cda_table" displayName="comforter_cda_table" ref="A1:F33" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:F33" xr:uid="{60EC4219-E3F1-48A9-8A10-9A735D5CAA88}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B3194266-B947-4321-8934-F9C47FA9DE1C}" name="Date" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{3BD6ED93-E3D0-4F67-BDB8-9FEC9229AD12}" name="Start Time" dataDxfId="4"/>
@@ -406,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1109,6 +1109,75 @@
         <v>35.000000000000036</v>
       </c>
     </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>43356</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0.84375</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.89097222222222217</v>
+      </c>
+      <c r="D31" s="3">
+        <f>(C31-B31)* 1440</f>
+        <v>67.999999999999915</v>
+      </c>
+      <c r="E31" s="4">
+        <f>IF(C31&gt;B31, (C31-B31)*1440, (B31-C31)*1440)</f>
+        <v>67.999999999999915</v>
+      </c>
+      <c r="F31" s="4">
+        <f>ABS((C31-B31)*1440)</f>
+        <v>67.999999999999915</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>43356</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.98402777777777783</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="D32" s="3">
+        <f>(C32-B32)* 1440</f>
+        <v>21.999999999999922</v>
+      </c>
+      <c r="E32" s="4">
+        <f>IF(C32&gt;B32, (C32-B32)*1440, (B32-C32)*1440)</f>
+        <v>21.999999999999922</v>
+      </c>
+      <c r="F32" s="4">
+        <f>ABS((C32-B32)*1440)</f>
+        <v>21.999999999999922</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>43357</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="D33" s="3">
+        <f>(C33-B33)* 1440</f>
+        <v>400</v>
+      </c>
+      <c r="E33" s="4">
+        <f>IF(C33&gt;B33, (C33-B33)*1440, (B33-C33)*1440)</f>
+        <v>400</v>
+      </c>
+      <c r="F33" s="4">
+        <f>ABS((C33-B33)*1440)</f>
+        <v>400</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add daily power updates
</commit_message>
<xml_diff>
--- a/pakuro/pakuro-cda.xlsx
+++ b/pakuro/pakuro-cda.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D365489-0171-44D8-A23F-820425AF6F85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A68E2A-714C-4D25-BE9D-6A5FE55E357A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="9000" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="9450" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="comforter-cda" sheetId="1" r:id="rId1"/>
@@ -123,8 +123,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4F241E2-70B8-4E1C-A71D-2175999E1A36}" name="comforter_cda_table" displayName="comforter_cda_table" ref="A1:F38" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:F38" xr:uid="{60EC4219-E3F1-48A9-8A10-9A735D5CAA88}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4F241E2-70B8-4E1C-A71D-2175999E1A36}" name="comforter_cda_table" displayName="comforter_cda_table" ref="A1:F41" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:F41" xr:uid="{60EC4219-E3F1-48A9-8A10-9A735D5CAA88}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B3194266-B947-4321-8934-F9C47FA9DE1C}" name="Date" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{3BD6ED93-E3D0-4F67-BDB8-9FEC9229AD12}" name="Start Time" dataDxfId="4"/>
@@ -406,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1293,6 +1293,63 @@
         <v>264</v>
       </c>
     </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>43363</v>
+      </c>
+      <c r="D39" s="3">
+        <f>(C39-B39)* 1440</f>
+        <v>0</v>
+      </c>
+      <c r="E39" s="4">
+        <f>IF(C39&gt;B39, (C39-B39)*1440, (B39-C39)*1440)</f>
+        <v>0</v>
+      </c>
+      <c r="F39" s="4">
+        <f>ABS((C39-B39)*1440)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>43364</v>
+      </c>
+      <c r="D40" s="3">
+        <f>(C40-B40)* 1440</f>
+        <v>0</v>
+      </c>
+      <c r="E40" s="4">
+        <f>IF(C40&gt;B40, (C40-B40)*1440, (B40-C40)*1440)</f>
+        <v>0</v>
+      </c>
+      <c r="F40" s="4">
+        <f>ABS((C40-B40)*1440)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>43365</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0.79583333333333339</v>
+      </c>
+      <c r="C41" s="1">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="D41" s="3">
+        <f>(C41-B41)* 1440</f>
+        <v>292.99999999999994</v>
+      </c>
+      <c r="E41" s="4">
+        <f>IF(C41&gt;B41, (C41-B41)*1440, (B41-C41)*1440)</f>
+        <v>292.99999999999994</v>
+      </c>
+      <c r="F41" s="4">
+        <f>ABS((C41-B41)*1440)</f>
+        <v>292.99999999999994</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>